<commit_message>
Setup and Initialize Workflow creation and processing.
Note there is unfinished code in this set, but I need to get it
controlled so I can fix a problem with Visual Paradigm

Signed-off-by: John Hetrick <hetrickjm@ornl.gov>
</commit_message>
<xml_diff>
--- a/org.eclipse.ice.modeling/docs/testData.xlsx
+++ b/org.eclipse.ice.modeling/docs/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ORNL\dev\git\iceJXH\org.eclipse.ice.modeling\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F93FCC0-89ED-4AD0-B0E7-8D5F3ECD744D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4C1784-CDDD-41DC-B83B-CA99127278AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="3660" windowWidth="19200" windowHeight="10073" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13" yWindow="3733" windowWidth="19200" windowHeight="10080" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSets" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="WorkflowDescr" sheetId="2" r:id="rId3"/>
     <sheet name="Tasks" sheetId="4" r:id="rId4"/>
     <sheet name="Map" sheetId="3" r:id="rId5"/>
+    <sheet name="Workflow" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>Instrument</t>
   </si>
@@ -241,6 +242,12 @@
     <t>NONE</t>
   </si>
   <si>
+    <t>INST-1/EXP-1/GRP-1/DT-2</t>
+  </si>
+  <si>
+    <t>INST-2/EXP-2/GRP-1/DT-0</t>
+  </si>
+  <si>
     <t>Seq Key</t>
   </si>
   <si>
@@ -265,25 +272,16 @@
     <t>INST-1/EXP-1/GRP-0/SEQ-0</t>
   </si>
   <si>
-    <t>INST-1/EXP-1/GRP-0/SEQ-0/DT-0</t>
-  </si>
-  <si>
-    <t>INST-1/EXP-1/GRP-0/SEQ-1/DT-0</t>
-  </si>
-  <si>
-    <t>INST-1/EXP-1/GRP-0/SEQ-2/DT-0</t>
-  </si>
-  <si>
-    <t>INST-1/EXP-1/GRP-1/SEQ-0/DT-2</t>
-  </si>
-  <si>
-    <t>INST-1/EXP-1/GRP-1/SEQ-2/DT-2</t>
-  </si>
-  <si>
-    <t>INST-1/EXP-1/GRP-1/SEQ-1/DT-2</t>
-  </si>
-  <si>
-    <t>INST-2/EXP-2/GRP-1/SEQ-1/DT-0</t>
+    <t>Note the Seq. number is not important for the key.  All sequences use the same workflow description</t>
+  </si>
+  <si>
+    <t>INST-1/EXP-1/GRP-0/DT-0/SEQ-0</t>
+  </si>
+  <si>
+    <t>INST-1/EXP-1/GRP-0/WFG-&lt;#&gt;</t>
+  </si>
+  <si>
+    <t>INST-1/EXP-1/GRP-0/WFS-&lt;#&gt;</t>
   </si>
 </sst>
 </file>
@@ -342,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -365,11 +363,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -377,6 +386,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +670,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -673,15 +683,15 @@
         <v>20</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
@@ -746,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -757,7 +767,7 @@
     <col min="4" max="4" width="9.64453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.46875" customWidth="1"/>
     <col min="7" max="7" width="29.234375" customWidth="1"/>
-    <col min="8" max="8" width="19.52734375" customWidth="1"/>
+    <col min="8" max="8" width="39.5859375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
@@ -777,10 +787,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
@@ -800,10 +810,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
         <v>62</v>
@@ -826,10 +836,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
@@ -849,10 +862,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.5">
@@ -872,10 +885,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
@@ -895,10 +908,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
@@ -918,10 +931,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
@@ -941,10 +954,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.5">
@@ -1573,12 +1586,12 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="23.46875" customWidth="1"/>
+    <col min="1" max="1" width="34.29296875" customWidth="1"/>
     <col min="2" max="3" width="20.17578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1604,7 +1617,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
@@ -1671,4 +1684,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003B03E4-0A76-40E5-B84E-83FE18B5E59A}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="28.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.46875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work on processing an incoming message. Handling new message indicating there is a data set ready for processing (reducing)
Signed-off-by: John Hetrick <hetrickjm@ornl.gov>
</commit_message>
<xml_diff>
--- a/org.eclipse.ice.modeling/docs/testData.xlsx
+++ b/org.eclipse.ice.modeling/docs/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ORNL\dev\git\iceJXH\org.eclipse.ice.modeling\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4C1784-CDDD-41DC-B83B-CA99127278AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532F9D7D-3A27-4614-A6D1-8F0EC9DFDD55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13" yWindow="3733" windowWidth="19200" windowHeight="10080" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3720" windowWidth="19200" windowHeight="10080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSets" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
   <si>
     <t>Instrument</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>INST-1/EXP-1/GRP-0/WFS-&lt;#&gt;</t>
+  </si>
+  <si>
+    <t>INST-1/EXP-1/GRP-0/DT-1</t>
   </si>
 </sst>
 </file>
@@ -756,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1092,12 +1095,12 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="20.9375" customWidth="1"/>
+    <col min="1" max="1" width="22.8203125" customWidth="1"/>
     <col min="4" max="4" width="14.1171875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.3515625" customWidth="1"/>
   </cols>
@@ -1130,7 +1133,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>27</v>
@@ -1154,7 +1157,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>28</v>
@@ -1362,7 +1365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B63730E-B6DD-4B44-9156-95F9B07D629B}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1690,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003B03E4-0A76-40E5-B84E-83FE18B5E59A}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>